<commit_message>
Update for new accessory
</commit_message>
<xml_diff>
--- a/_extensions/bemer-invoice/prix original.xlsx
+++ b/_extensions/bemer-invoice/prix original.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandineburkhard/Dropbox/BEMER/BemerDoc/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pascalburkhard/Library/CloudStorage/Dropbox/Private/BEMER/BemerDoc/_extensions/nenuial/bemer-invoice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9F655C-3F8C-0347-BB7D-ED2B5FF1C2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51525222-0B97-D044-BEA6-C7C00CBD4B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="12240" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="900" windowWidth="17100" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>ref</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Couverture séchante</t>
+  </si>
+  <si>
+    <t>Applicateur d'encolure</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -183,7 +186,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -202,7 +204,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -498,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,7 +531,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -615,509 +617,529 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>423500</v>
+        <v>423700</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1">
-        <v>2550</v>
+        <v>2190</v>
       </c>
       <c r="D6" s="1">
-        <v>2605</v>
+        <v>2190</v>
       </c>
       <c r="E6" s="1">
-        <v>1912.5</v>
+        <v>1642.5</v>
       </c>
       <c r="F6" s="3">
-        <v>845</v>
+        <v>775</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>420100</v>
+        <v>423500</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1">
-        <v>2390</v>
+        <v>2550</v>
       </c>
       <c r="D7" s="1">
-        <v>2310</v>
+        <v>2605</v>
       </c>
       <c r="E7" s="1">
-        <v>1792.5</v>
+        <v>1912.5</v>
       </c>
       <c r="F7" s="3">
-        <v>735</v>
+        <v>845</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>420200</v>
+        <v>420100</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1">
-        <v>3360</v>
+        <v>2390</v>
       </c>
       <c r="D8" s="1">
-        <v>3225</v>
+        <v>2310</v>
       </c>
       <c r="E8" s="1">
-        <v>2520</v>
+        <v>1792.5</v>
       </c>
       <c r="F8" s="3">
-        <v>1040</v>
+        <v>735</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>430100</v>
+        <v>420200</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1">
-        <v>560</v>
+        <v>3360</v>
       </c>
       <c r="D9" s="1">
-        <v>510</v>
+        <v>3225</v>
       </c>
       <c r="E9" s="1">
-        <v>420</v>
+        <v>2520</v>
       </c>
       <c r="F9" s="3">
-        <v>160</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>430200</v>
+        <v>430100</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="D10" s="1">
-        <v>540</v>
+        <v>510</v>
       </c>
       <c r="E10" s="1">
-        <v>423.75</v>
+        <v>420</v>
       </c>
       <c r="F10" s="3">
-        <v>175</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>430300</v>
+        <v>430200</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1">
-        <v>236</v>
+        <v>565</v>
       </c>
       <c r="D11" s="1">
-        <v>235</v>
+        <v>540</v>
       </c>
       <c r="E11" s="1">
-        <v>177</v>
+        <v>423.75</v>
       </c>
       <c r="F11" s="3">
-        <v>75</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>431000</v>
+        <v>430300</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1">
-        <v>113</v>
+        <v>236</v>
       </c>
       <c r="D12" s="1">
-        <v>110</v>
+        <v>235</v>
       </c>
       <c r="E12" s="1">
-        <v>84.75</v>
+        <v>177</v>
       </c>
       <c r="F12" s="3">
-        <v>35</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>431100</v>
+        <v>431000</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1">
-        <v>170</v>
+        <v>113</v>
       </c>
       <c r="D13" s="1">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="E13" s="1">
-        <v>127.5</v>
+        <v>84.75</v>
       </c>
       <c r="F13" s="3">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>431200</v>
+        <v>431100</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1">
-        <v>435</v>
+        <v>170</v>
       </c>
       <c r="D14" s="1">
-        <v>415</v>
+        <v>165</v>
       </c>
       <c r="E14" s="1">
-        <v>326.25</v>
+        <v>127.5</v>
       </c>
       <c r="F14" s="3">
-        <v>135</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>431400</v>
+        <v>431200</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1">
-        <v>470</v>
+        <v>435</v>
       </c>
       <c r="D15" s="1">
-        <v>455</v>
+        <v>415</v>
       </c>
       <c r="E15" s="1">
-        <v>352.5</v>
+        <v>326.25</v>
       </c>
       <c r="F15" s="3">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>440100</v>
+        <v>431400</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1">
-        <v>86</v>
+        <v>470</v>
       </c>
       <c r="D16" s="1">
-        <v>83</v>
+        <v>455</v>
       </c>
       <c r="E16" s="1">
-        <v>73.099999999999994</v>
+        <v>352.5</v>
+      </c>
+      <c r="F16" s="3">
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>440200</v>
+        <v>440100</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1">
-        <v>154</v>
+        <v>86</v>
       </c>
       <c r="D17" s="1">
-        <v>153</v>
+        <v>83</v>
       </c>
       <c r="E17" s="1">
-        <v>130.9</v>
+        <v>73.099999999999994</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>440300</v>
+        <v>440200</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1">
-        <v>24.5</v>
+        <v>154</v>
       </c>
       <c r="D18" s="1">
-        <v>22.5</v>
+        <v>153</v>
       </c>
       <c r="E18" s="1">
-        <v>20.83</v>
+        <v>130.9</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>450100</v>
+        <v>440300</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1">
-        <v>47</v>
+        <v>24.5</v>
       </c>
       <c r="D19" s="1">
-        <v>46</v>
+        <v>22.5</v>
       </c>
       <c r="E19" s="1">
-        <v>39.950000000000003</v>
+        <v>20.83</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>450200</v>
+        <v>450100</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1">
-        <v>38.5</v>
+        <v>47</v>
       </c>
       <c r="D20" s="1">
-        <v>34.5</v>
+        <v>46</v>
       </c>
       <c r="E20" s="1">
-        <v>32.729999999999997</v>
+        <v>39.950000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>450600</v>
+        <v>450200</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1">
-        <v>32</v>
+        <v>38.5</v>
       </c>
       <c r="D21" s="1">
-        <v>29.5</v>
+        <v>34.5</v>
       </c>
       <c r="E21" s="1">
-        <v>27.2</v>
+        <v>32.729999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>455000</v>
+        <v>450600</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1">
-        <v>94.5</v>
+        <v>32</v>
       </c>
       <c r="D22" s="1">
-        <v>94</v>
+        <v>29.5</v>
       </c>
       <c r="E22" s="1">
-        <v>80.33</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>450700</v>
+        <v>455000</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1">
-        <v>19</v>
+        <v>94.5</v>
       </c>
       <c r="D23" s="1">
-        <v>17.5</v>
+        <v>94</v>
       </c>
       <c r="E23" s="1">
-        <v>16.149999999999999</v>
+        <v>80.33</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>457000</v>
+        <v>450700</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C24" s="1">
-        <v>77.5</v>
+        <v>19</v>
       </c>
       <c r="D24" s="1">
-        <v>75</v>
+        <v>17.5</v>
       </c>
       <c r="E24" s="1">
-        <v>68.87</v>
+        <v>16.149999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>450800</v>
+        <v>457000</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1">
-        <v>38.5</v>
+        <v>77.5</v>
       </c>
       <c r="D25" s="1">
-        <v>34.5</v>
+        <v>75</v>
       </c>
       <c r="E25" s="1">
-        <v>32.729999999999997</v>
+        <v>68.87</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>452000</v>
+        <v>450800</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C26" s="1">
-        <v>43.5</v>
+        <v>38.5</v>
       </c>
       <c r="D26" s="1">
-        <v>40.5</v>
+        <v>34.5</v>
       </c>
       <c r="E26" s="1">
-        <v>36.979999999999997</v>
+        <v>32.729999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>452100</v>
+        <v>452000</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1">
-        <v>67</v>
+        <v>43.5</v>
       </c>
       <c r="D27" s="1">
-        <v>65</v>
+        <v>40.5</v>
       </c>
       <c r="E27" s="1">
-        <v>56.95</v>
+        <v>36.979999999999997</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>455300</v>
+        <v>452100</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1">
-        <v>173</v>
+        <v>67</v>
       </c>
       <c r="D28" s="1">
-        <v>174</v>
+        <v>65</v>
       </c>
       <c r="E28" s="1">
-        <v>147.05000000000001</v>
+        <v>56.95</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>422800</v>
+        <v>455300</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D29" s="1">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="E29" s="1">
-        <v>152.15</v>
-      </c>
-      <c r="F29" s="3"/>
+        <v>147.05000000000001</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>423600</v>
+        <v>422800</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C30" s="1">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="D30" s="1">
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="E30" s="1">
-        <v>128.35</v>
+        <v>152.15</v>
       </c>
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>459000</v>
+        <v>423600</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="D31" s="1">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="E31" s="1">
-        <v>114.75</v>
-      </c>
+        <v>128.35</v>
+      </c>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>440900</v>
+        <v>459000</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="D32" s="1">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="E32" s="1">
-        <v>135.15</v>
+        <v>114.75</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
+        <v>440900</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="1">
+        <v>159</v>
+      </c>
+      <c r="D33" s="1">
+        <v>157</v>
+      </c>
+      <c r="E33" s="1">
+        <v>135.15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>440950</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C34" s="1">
         <v>83</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D34" s="1">
         <v>83</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E34" s="1">
         <v>70.55</v>
       </c>
     </row>

</xml_diff>